<commit_message>
few changes to data dictonary thing
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="99">
   <si>
     <t>Entity</t>
   </si>
@@ -111,18 +111,9 @@
     <t>Number(4,1)</t>
   </si>
   <si>
-    <t>Check (Length &gt;= 0)</t>
-  </si>
-  <si>
-    <t>Check (Length &gt;=0)</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Default 0</t>
-  </si>
-  <si>
     <t>Foreign Key(LOC_BUILDING_FK)</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>Foreign Key</t>
   </si>
   <si>
-    <t>Check (Quantity &gt;= 0)</t>
-  </si>
-  <si>
     <t>PC Allocation</t>
   </si>
   <si>
@@ -310,6 +298,21 @@
   </si>
   <si>
     <t>Homephone</t>
+  </si>
+  <si>
+    <t>Check (Length &gt;= 0), Default 0</t>
+  </si>
+  <si>
+    <t>Check (Length &gt;=0), Default 0</t>
+  </si>
+  <si>
+    <t>Check (Quantity &gt;= 0), Default 0</t>
+  </si>
+  <si>
+    <t>EventDate</t>
+  </si>
+  <si>
+    <t>Default Sysdate</t>
   </si>
 </sst>
 </file>
@@ -368,16 +371,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,11 +682,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,16 +697,16 @@
     <col min="5" max="5" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
     <col min="10" max="10" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -719,21 +722,21 @@
       <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>85</v>
+      <c r="H1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -751,8 +754,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -760,18 +763,18 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -779,15 +782,15 @@
         <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
@@ -795,15 +798,15 @@
         <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -811,17 +814,17 @@
         <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -832,15 +835,15 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
@@ -848,15 +851,15 @@
         <v>27</v>
       </c>
       <c r="I10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
@@ -864,15 +867,15 @@
         <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
@@ -880,15 +883,15 @@
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
@@ -896,15 +899,15 @@
         <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
@@ -912,21 +915,18 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
@@ -934,21 +934,18 @@
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
@@ -956,20 +953,20 @@
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="3"/>
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
@@ -977,97 +974,97 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="D19" t="s">
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+      <c r="J19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" t="s">
+        <v>83</v>
+      </c>
+      <c r="J21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I19" t="s">
-        <v>87</v>
-      </c>
-      <c r="J19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" t="s">
-        <v>87</v>
-      </c>
-      <c r="J20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" t="s">
         <v>51</v>
       </c>
-      <c r="F23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="I24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1075,65 +1072,65 @@
         <v>12</v>
       </c>
       <c r="I25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J25" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
       <c r="I26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" t="s">
         <v>44</v>
       </c>
-      <c r="J26" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" t="s">
-        <v>50</v>
-      </c>
       <c r="I27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J28" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="3"/>
+      <c r="A30" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="7"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1141,78 +1138,75 @@
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="J32" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J35" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="1" t="s">
         <v>20</v>
       </c>
@@ -1220,110 +1214,113 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="3"/>
+      <c r="A38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="7"/>
       <c r="C38" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
         <v>28</v>
       </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
       <c r="I39" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
       </c>
       <c r="I40" t="s">
+        <v>59</v>
+      </c>
+      <c r="J40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" t="s">
+        <v>59</v>
+      </c>
+      <c r="J41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J40" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D41" t="s">
-        <v>62</v>
-      </c>
-      <c r="I41" t="s">
-        <v>63</v>
-      </c>
-      <c r="J41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J42" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
       </c>
       <c r="I43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J43" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
       <c r="C44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1331,31 +1328,31 @@
         <v>28</v>
       </c>
       <c r="I44" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I45" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J45" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
       <c r="C46" s="1" t="s">
         <v>20</v>
       </c>
@@ -1363,85 +1360,85 @@
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B48" s="3"/>
+      <c r="A48" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="7"/>
       <c r="C48" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F48" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
       <c r="C49" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
       <c r="C50" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D51" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="3"/>
+      <c r="A55" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="7"/>
       <c r="C55" s="1" t="s">
         <v>20</v>
       </c>
@@ -1449,54 +1446,70 @@
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="E57" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
       <c r="C58" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A55:B58"/>
-    <mergeCell ref="A30:B32"/>
-    <mergeCell ref="A34:B36"/>
-    <mergeCell ref="A38:B46"/>
-    <mergeCell ref="A48:B53"/>
+    <mergeCell ref="A55:B59"/>
     <mergeCell ref="A23:B28"/>
     <mergeCell ref="A3:B7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B16"/>
     <mergeCell ref="A18:B21"/>
+    <mergeCell ref="A30:B32"/>
+    <mergeCell ref="A34:B36"/>
+    <mergeCell ref="A38:B46"/>
+    <mergeCell ref="A48:B53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added defaults in both database creation script and the data dictionary
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="113">
   <si>
     <t>Entity</t>
   </si>
@@ -174,9 +174,6 @@
     <t>EQUIPMENT_SEC</t>
   </si>
   <si>
-    <t>Equipment Allocation</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -300,21 +297,6 @@
     <t>Homephone</t>
   </si>
   <si>
-    <t>Check (Length &gt;= 0), Default 0</t>
-  </si>
-  <si>
-    <t>Check (Length &gt;=0), Default 0</t>
-  </si>
-  <si>
-    <t>Check (Quantity &gt;= 0), Default 0</t>
-  </si>
-  <si>
-    <t>EventDate</t>
-  </si>
-  <si>
-    <t>Default Sysdate</t>
-  </si>
-  <si>
     <t>Each pc only has one entry in the 3 columns, this entry is used</t>
   </si>
   <si>
@@ -354,7 +336,25 @@
     <t>End time</t>
   </si>
   <si>
-    <t xml:space="preserve">Booking </t>
+    <t>Equipment    Allocation</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Check (Length &gt;=0)</t>
+  </si>
+  <si>
+    <t>Check (Length &gt;= 0)</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>sysdate</t>
+  </si>
+  <si>
+    <t>Check (Quantity &gt;= 0)</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -422,6 +422,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,28 +733,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="29.5703125" customWidth="1"/>
-    <col min="11" max="11" width="55.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.5703125" customWidth="1"/>
+    <col min="12" max="12" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -759,26 +770,29 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -792,23 +806,23 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="J3" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
@@ -820,14 +834,14 @@
       <c r="E4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" t="s">
-        <v>80</v>
-      </c>
       <c r="J4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
@@ -836,14 +850,17 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
-        <v>80</v>
+      <c r="F5" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="1" t="s">
@@ -852,14 +869,17 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s">
-        <v>80</v>
+      <c r="F6" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="1" t="s">
@@ -868,14 +888,17 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="s">
-        <v>80</v>
+      <c r="F7" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="K7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
@@ -889,23 +912,23 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="J9" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="1" t="s">
@@ -914,14 +937,17 @@
       <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="I10" t="s">
-        <v>83</v>
+      <c r="F10" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
@@ -930,14 +956,17 @@
       <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="I11" t="s">
+      <c r="F11" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" t="s">
         <v>83</v>
       </c>
-      <c r="J11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="1" t="s">
@@ -946,14 +975,17 @@
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="I12" t="s">
-        <v>83</v>
+      <c r="F12" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="1" t="s">
@@ -962,14 +994,17 @@
       <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="I13" t="s">
-        <v>83</v>
+      <c r="F13" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="1" t="s">
@@ -979,16 +1014,19 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>83</v>
+        <v>109</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
       </c>
       <c r="J14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="1" t="s">
@@ -998,16 +1036,19 @@
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>83</v>
+        <v>108</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0</v>
       </c>
       <c r="J15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="1" t="s">
@@ -1019,14 +1060,17 @@
       <c r="E16" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="6" t="s">
-        <v>83</v>
+      <c r="F16" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J16" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
@@ -1040,17 +1084,17 @@
       <c r="E18" t="s">
         <v>40</v>
       </c>
-      <c r="I18" t="s">
-        <v>101</v>
-      </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="1" t="s">
@@ -1059,14 +1103,17 @@
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="I19" t="s">
-        <v>83</v>
+      <c r="F19" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="1" t="s">
@@ -1075,14 +1122,17 @@
       <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="I20" t="s">
-        <v>83</v>
+      <c r="F20" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="1" t="s">
@@ -1091,14 +1141,17 @@
       <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="I21" t="s">
-        <v>83</v>
+      <c r="F21" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>41</v>
       </c>
@@ -1112,23 +1165,23 @@
       <c r="E23" t="s">
         <v>48</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>49</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>51</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="J23" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="1" t="s">
@@ -1137,14 +1190,17 @@
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="I24" t="s">
+      <c r="F24" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" t="s">
         <v>41</v>
       </c>
-      <c r="J24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="1" t="s">
@@ -1153,14 +1209,17 @@
       <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="I25" t="s">
+      <c r="F25" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J25" t="s">
         <v>41</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="1" t="s">
@@ -1169,14 +1228,17 @@
       <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="I26" t="s">
+      <c r="F26" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J26" t="s">
         <v>41</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="1" t="s">
@@ -1185,14 +1247,17 @@
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="I27" t="s">
+      <c r="F27" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J27" t="s">
         <v>41</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="1" t="s">
@@ -1201,18 +1266,21 @@
       <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="I28" t="s">
+      <c r="F28" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J28" t="s">
         <v>41</v>
       </c>
-      <c r="J28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="7"/>
+      <c r="K28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="9"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1222,19 +1290,19 @@
       <c r="E30" t="s">
         <v>40</v>
       </c>
-      <c r="I30" t="s">
-        <v>101</v>
-      </c>
       <c r="J30" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
+        <v>95</v>
+      </c>
+      <c r="L30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
       <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1244,42 +1312,45 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
-      <c r="I31" t="s">
-        <v>101</v>
-      </c>
       <c r="J31" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+        <v>95</v>
+      </c>
+      <c r="L31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
       <c r="C32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>96</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>83</v>
+        <v>112</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -1287,36 +1358,39 @@
       <c r="E34" t="s">
         <v>48</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
+        <v>89</v>
+      </c>
+      <c r="K34" t="s">
         <v>90</v>
       </c>
-      <c r="J34" t="s">
-        <v>91</v>
-      </c>
-      <c r="K34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" t="s">
         <v>57</v>
       </c>
-      <c r="D35" t="s">
-        <v>58</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="F35" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35" t="s">
         <v>90</v>
       </c>
-      <c r="J35" t="s">
-        <v>91</v>
-      </c>
-      <c r="K35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="1" t="s">
@@ -1326,25 +1400,28 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
-      </c>
-      <c r="I36" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J36" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -1352,20 +1429,20 @@
       <c r="E38" t="s">
         <v>48</v>
       </c>
-      <c r="F38" t="s">
-        <v>67</v>
-      </c>
-      <c r="I38" s="6" t="s">
-        <v>101</v>
+      <c r="G38" t="s">
+        <v>66</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="1" t="s">
@@ -1377,78 +1454,93 @@
       <c r="E39" t="s">
         <v>39</v>
       </c>
-      <c r="I39" t="s">
-        <v>59</v>
+      <c r="F39" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J39" t="s">
+        <v>58</v>
+      </c>
+      <c r="K39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
       </c>
-      <c r="I40" t="s">
-        <v>59</v>
+      <c r="F40" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J41" t="s">
         <v>58</v>
       </c>
-      <c r="I41" t="s">
-        <v>59</v>
-      </c>
-      <c r="J41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J42" t="s">
         <v>58</v>
       </c>
-      <c r="I42" t="s">
-        <v>59</v>
-      </c>
-      <c r="J42" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
       </c>
-      <c r="I43" t="s">
-        <v>59</v>
+      <c r="F43" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J43" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="1" t="s">
@@ -1457,30 +1549,36 @@
       <c r="D44" t="s">
         <v>28</v>
       </c>
-      <c r="I44" t="s">
-        <v>59</v>
+      <c r="F44" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J44" t="s">
+        <v>58</v>
+      </c>
+      <c r="K44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
         <v>65</v>
       </c>
-      <c r="D45" t="s">
-        <v>66</v>
-      </c>
-      <c r="I45" t="s">
-        <v>59</v>
+      <c r="F45" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K45" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="1" t="s">
@@ -1490,16 +1588,19 @@
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -1507,111 +1608,126 @@
       <c r="E48" t="s">
         <v>48</v>
       </c>
-      <c r="F48" t="s">
-        <v>74</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>101</v>
+      <c r="G48" t="s">
+        <v>73</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D49" t="s">
         <v>28</v>
       </c>
-      <c r="I49" s="6" t="s">
-        <v>101</v>
+      <c r="F49" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="L49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s">
         <v>28</v>
       </c>
-      <c r="I50" s="6" t="s">
-        <v>75</v>
+      <c r="F50" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" t="s">
         <v>28</v>
       </c>
-      <c r="I51" s="6" t="s">
-        <v>75</v>
+      <c r="F51" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
-      <c r="I52" s="6" t="s">
-        <v>75</v>
+      <c r="F52" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>54</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>101</v>
+        <v>53</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K53" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="L53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="1" t="s">
@@ -1623,21 +1739,21 @@
       <c r="E55" t="s">
         <v>40</v>
       </c>
-      <c r="I55" t="s">
-        <v>101</v>
-      </c>
       <c r="J55" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K55" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -1645,73 +1761,61 @@
       <c r="E56" t="s">
         <v>40</v>
       </c>
-      <c r="I56" t="s">
-        <v>101</v>
-      </c>
       <c r="J56" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K56" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="L56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D57" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" t="s">
-        <v>98</v>
-      </c>
-      <c r="I57" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="J57" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K57" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" t="s">
         <v>77</v>
       </c>
-      <c r="D58" t="s">
-        <v>78</v>
-      </c>
-      <c r="I58" t="s">
-        <v>75</v>
+      <c r="F58" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="J58" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D59" t="s">
-        <v>78</v>
-      </c>
-      <c r="E59" t="s">
-        <v>98</v>
-      </c>
-      <c r="I59" t="s">
-        <v>112</v>
-      </c>
-      <c r="J59" t="s">
-        <v>78</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="K58" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A55:B59"/>
     <mergeCell ref="A23:B28"/>
     <mergeCell ref="A3:B7"/>
     <mergeCell ref="A1:B1"/>
@@ -1721,6 +1825,7 @@
     <mergeCell ref="A34:B36"/>
     <mergeCell ref="A38:B46"/>
     <mergeCell ref="A48:B53"/>
+    <mergeCell ref="A55:B58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed a query, and added beginnings of several documentation pieces
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="117">
   <si>
     <t>Entity</t>
   </si>
@@ -355,6 +355,18 @@
   </si>
   <si>
     <t>Check (Quantity &gt;= 0)</t>
+  </si>
+  <si>
+    <t>Comments/Purpose</t>
+  </si>
+  <si>
+    <t>To provide a unique ID for the Building table</t>
+  </si>
+  <si>
+    <t>Storing the name of the building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storing the campus that the building is located at </t>
   </si>
 </sst>
 </file>
@@ -407,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -417,6 +429,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,11 +444,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,8 +751,8 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,20 +762,20 @@
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="4" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="29.5703125" customWidth="1"/>
     <col min="12" max="12" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -770,7 +785,7 @@
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -780,7 +795,7 @@
         <v>17</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>78</v>
@@ -792,11 +807,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -812,6 +827,9 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
+      <c r="I3" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="J3" s="6" t="s">
         <v>95</v>
       </c>
@@ -822,9 +840,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -834,6 +852,9 @@
       <c r="E4" t="s">
         <v>39</v>
       </c>
+      <c r="I4" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="J4" t="s">
         <v>79</v>
       </c>
@@ -841,17 +862,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>110</v>
+      <c r="F5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="J5" t="s">
         <v>79</v>
@@ -861,17 +885,18 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="12"/>
       <c r="J6" t="s">
         <v>79</v>
       </c>
@@ -880,17 +905,18 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="12"/>
       <c r="J7" t="s">
         <v>79</v>
       </c>
@@ -898,11 +924,14 @@
         <v>81</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8" s="12"/>
+    </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -918,6 +947,7 @@
       <c r="H9" t="s">
         <v>50</v>
       </c>
+      <c r="I9" s="12"/>
       <c r="J9" s="6" t="s">
         <v>95</v>
       </c>
@@ -929,17 +959,18 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="12"/>
       <c r="J10" t="s">
         <v>82</v>
       </c>
@@ -948,17 +979,18 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F11" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="12"/>
       <c r="J11" t="s">
         <v>82</v>
       </c>
@@ -967,17 +999,18 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F12" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I12" s="12"/>
       <c r="J12" t="s">
         <v>82</v>
       </c>
@@ -986,17 +1019,18 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F13" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I13" s="12"/>
       <c r="J13" t="s">
         <v>82</v>
       </c>
@@ -1005,8 +1039,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1016,9 +1050,10 @@
       <c r="E14" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <v>0</v>
       </c>
+      <c r="I14" s="12"/>
       <c r="J14" s="6" t="s">
         <v>82</v>
       </c>
@@ -1027,8 +1062,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1038,9 +1073,10 @@
       <c r="E15" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F15" s="8">
         <v>0</v>
       </c>
+      <c r="I15" s="12"/>
       <c r="J15" s="6" t="s">
         <v>82</v>
       </c>
@@ -1049,8 +1085,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1060,9 +1096,10 @@
       <c r="E16" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F16" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="12"/>
       <c r="J16" s="6" t="s">
         <v>82</v>
       </c>
@@ -1070,11 +1107,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I17" s="12"/>
+    </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1084,6 +1124,7 @@
       <c r="E18" t="s">
         <v>40</v>
       </c>
+      <c r="I18" s="12"/>
       <c r="J18" t="s">
         <v>95</v>
       </c>
@@ -1095,17 +1136,18 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
       <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D19" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F19" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I19" s="12"/>
       <c r="J19" t="s">
         <v>82</v>
       </c>
@@ -1114,17 +1156,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" s="12"/>
       <c r="J20" t="s">
         <v>82</v>
       </c>
@@ -1133,17 +1176,18 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F21" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" s="12"/>
       <c r="J21" t="s">
         <v>82</v>
       </c>
@@ -1151,11 +1195,14 @@
         <v>86</v>
       </c>
     </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I22" s="12"/>
+    </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1171,6 +1218,7 @@
       <c r="H23" t="s">
         <v>51</v>
       </c>
+      <c r="I23" s="12"/>
       <c r="J23" s="6" t="s">
         <v>95</v>
       </c>
@@ -1182,17 +1230,18 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="12"/>
       <c r="J24" t="s">
         <v>41</v>
       </c>
@@ -1201,17 +1250,18 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F25" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I25" s="12"/>
       <c r="J25" t="s">
         <v>41</v>
       </c>
@@ -1220,17 +1270,18 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
       <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="12"/>
       <c r="J26" t="s">
         <v>41</v>
       </c>
@@ -1239,17 +1290,18 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F27" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="12"/>
       <c r="J27" t="s">
         <v>41</v>
       </c>
@@ -1258,17 +1310,18 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I28" s="12"/>
       <c r="J28" t="s">
         <v>41</v>
       </c>
@@ -1276,11 +1329,14 @@
         <v>88</v>
       </c>
     </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I29" s="12"/>
+    </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1290,6 +1346,7 @@
       <c r="E30" t="s">
         <v>40</v>
       </c>
+      <c r="I30" s="12"/>
       <c r="J30" t="s">
         <v>95</v>
       </c>
@@ -1301,8 +1358,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1312,6 +1369,7 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
+      <c r="I31" s="12"/>
       <c r="J31" t="s">
         <v>95</v>
       </c>
@@ -1323,8 +1381,8 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="1" t="s">
         <v>52</v>
       </c>
@@ -1334,9 +1392,10 @@
       <c r="E32" t="s">
         <v>112</v>
       </c>
-      <c r="F32" s="11">
+      <c r="F32" s="8">
         <v>0</v>
       </c>
+      <c r="I32" s="12"/>
       <c r="J32" s="6" t="s">
         <v>82</v>
       </c>
@@ -1344,11 +1403,14 @@
         <v>52</v>
       </c>
     </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I33" s="12"/>
+    </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="1" t="s">
         <v>55</v>
       </c>
@@ -1358,6 +1420,7 @@
       <c r="E34" t="s">
         <v>48</v>
       </c>
+      <c r="I34" s="12"/>
       <c r="J34" t="s">
         <v>89</v>
       </c>
@@ -1369,17 +1432,18 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
       <c r="C35" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D35" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F35" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I35" s="12"/>
       <c r="J35" t="s">
         <v>89</v>
       </c>
@@ -1391,8 +1455,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
       <c r="C36" s="1" t="s">
         <v>20</v>
       </c>
@@ -1402,9 +1466,10 @@
       <c r="E36" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F36" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I36" s="12"/>
       <c r="J36" t="s">
         <v>95</v>
       </c>
@@ -1415,11 +1480,14 @@
         <v>96</v>
       </c>
     </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I37" s="12"/>
+    </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="1" t="s">
         <v>59</v>
       </c>
@@ -1432,6 +1500,7 @@
       <c r="G38" t="s">
         <v>66</v>
       </c>
+      <c r="I38" s="12"/>
       <c r="J38" s="6" t="s">
         <v>95</v>
       </c>
@@ -1443,8 +1512,8 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1454,9 +1523,10 @@
       <c r="E39" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F39" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39" s="12"/>
       <c r="J39" t="s">
         <v>58</v>
       </c>
@@ -1465,17 +1535,18 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D40" t="s">
         <v>28</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F40" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I40" s="12"/>
       <c r="J40" t="s">
         <v>58</v>
       </c>
@@ -1484,17 +1555,18 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D41" t="s">
         <v>57</v>
       </c>
-      <c r="F41" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F41" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I41" s="12"/>
       <c r="J41" t="s">
         <v>58</v>
       </c>
@@ -1503,17 +1575,18 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D42" t="s">
         <v>57</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F42" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I42" s="12"/>
       <c r="J42" t="s">
         <v>58</v>
       </c>
@@ -1522,17 +1595,18 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D43" t="s">
         <v>28</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F43" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I43" s="12"/>
       <c r="J43" t="s">
         <v>58</v>
       </c>
@@ -1541,17 +1615,18 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
       </c>
-      <c r="F44" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F44" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I44" s="12"/>
       <c r="J44" t="s">
         <v>58</v>
       </c>
@@ -1560,17 +1635,18 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D45" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F45" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" s="12"/>
       <c r="J45" t="s">
         <v>58</v>
       </c>
@@ -1579,8 +1655,8 @@
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
       <c r="C46" s="1" t="s">
         <v>20</v>
       </c>
@@ -1590,15 +1666,19 @@
       <c r="E46" t="s">
         <v>53</v>
       </c>
-      <c r="F46" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F46" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I46" s="12"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I47" s="12"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="9"/>
       <c r="C48" s="1" t="s">
         <v>68</v>
       </c>
@@ -1611,6 +1691,7 @@
       <c r="G48" t="s">
         <v>73</v>
       </c>
+      <c r="I48" s="12"/>
       <c r="J48" s="6" t="s">
         <v>95</v>
       </c>
@@ -1622,17 +1703,18 @@
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D49" t="s">
         <v>28</v>
       </c>
-      <c r="F49" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F49" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I49" s="12"/>
       <c r="J49" s="6" t="s">
         <v>95</v>
       </c>
@@ -1644,17 +1726,18 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
       <c r="C50" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D50" t="s">
         <v>28</v>
       </c>
-      <c r="F50" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F50" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" s="12"/>
       <c r="J50" s="6" t="s">
         <v>74</v>
       </c>
@@ -1663,17 +1746,18 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
       <c r="C51" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D51" t="s">
         <v>28</v>
       </c>
-      <c r="F51" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F51" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I51" s="12"/>
       <c r="J51" s="6" t="s">
         <v>74</v>
       </c>
@@ -1682,17 +1766,18 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
       <c r="C52" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F52" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I52" s="12"/>
       <c r="J52" s="6" t="s">
         <v>74</v>
       </c>
@@ -1701,8 +1786,8 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
       <c r="C53" s="1" t="s">
         <v>59</v>
       </c>
@@ -1712,9 +1797,10 @@
       <c r="E53" t="s">
         <v>53</v>
       </c>
-      <c r="F53" s="11" t="s">
-        <v>110</v>
-      </c>
+      <c r="F53" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I53" s="12"/>
       <c r="J53" s="6" t="s">
         <v>95</v>
       </c>
@@ -1725,11 +1811,14 @@
         <v>102</v>
       </c>
     </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I54" s="12"/>
+    </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="7"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="1" t="s">
         <v>20</v>
       </c>
@@ -1739,6 +1828,7 @@
       <c r="E55" t="s">
         <v>40</v>
       </c>
+      <c r="I55" s="12"/>
       <c r="J55" t="s">
         <v>95</v>
       </c>
@@ -1750,8 +1840,8 @@
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
       <c r="C56" s="1" t="s">
         <v>68</v>
       </c>
@@ -1761,6 +1851,7 @@
       <c r="E56" t="s">
         <v>40</v>
       </c>
+      <c r="I56" s="12"/>
       <c r="J56" t="s">
         <v>95</v>
       </c>
@@ -1772,17 +1863,18 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
       <c r="C57" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D57" t="s">
         <v>77</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="8" t="s">
         <v>111</v>
       </c>
+      <c r="I57" s="12"/>
       <c r="J57" t="s">
         <v>74</v>
       </c>
@@ -1791,17 +1883,18 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
       <c r="C58" s="1" t="s">
         <v>76</v>
       </c>
       <c r="D58" t="s">
         <v>77</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="8" t="s">
         <v>111</v>
       </c>
+      <c r="I58" s="12"/>
       <c r="J58" t="s">
         <v>74</v>
       </c>
@@ -1816,16 +1909,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A30:B32"/>
+    <mergeCell ref="A34:B36"/>
+    <mergeCell ref="A38:B46"/>
+    <mergeCell ref="A48:B53"/>
+    <mergeCell ref="A55:B58"/>
     <mergeCell ref="A23:B28"/>
     <mergeCell ref="A3:B7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B16"/>
     <mergeCell ref="A18:B21"/>
-    <mergeCell ref="A30:B32"/>
-    <mergeCell ref="A34:B36"/>
-    <mergeCell ref="A38:B46"/>
-    <mergeCell ref="A48:B53"/>
-    <mergeCell ref="A55:B58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished the Database Specification Comments
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="113">
   <si>
     <t>Entity</t>
   </si>
@@ -226,9 +226,6 @@
   </si>
   <si>
     <t>Faculty</t>
-  </si>
-  <si>
-    <t>Organiser</t>
   </si>
   <si>
     <t>EVENT_TRIG</t>
@@ -424,18 +421,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,11 +734,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G54" sqref="G54"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,10 +757,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -774,7 +771,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
@@ -782,24 +779,24 @@
       <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>76</v>
+      <c r="I1" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I2" s="11"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -815,19 +812,19 @@
       <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>93</v>
+      <c r="I3" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -837,16 +834,16 @@
       <c r="E4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>77</v>
+      <c r="I4" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -854,18 +851,18 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>77</v>
+        <v>107</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
@@ -873,18 +870,18 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>77</v>
+        <v>107</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -892,23 +889,23 @@
         <v>13</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>77</v>
+        <v>107</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I8" s="11"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -924,19 +921,19 @@
       <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>93</v>
+      <c r="I9" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
@@ -944,18 +941,18 @@
         <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
@@ -963,18 +960,18 @@
         <v>28</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I11" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" t="s">
         <v>80</v>
       </c>
-      <c r="J11" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
@@ -982,18 +979,18 @@
         <v>29</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1001,18 +998,18 @@
         <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1020,21 +1017,21 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
       </c>
-      <c r="I14" s="12" t="s">
-        <v>80</v>
+      <c r="I14" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1042,21 +1039,21 @@
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>80</v>
+      <c r="I15" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1067,23 +1064,23 @@
         <v>32</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I17" s="11"/>
+      <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1093,19 +1090,19 @@
       <c r="E18" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" t="s">
+        <v>92</v>
+      </c>
+      <c r="K18" t="s">
         <v>93</v>
       </c>
-      <c r="J18" t="s">
-        <v>93</v>
-      </c>
-      <c r="K18" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1113,18 +1110,18 @@
         <v>38</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1132,18 +1129,18 @@
         <v>38</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1151,23 +1148,23 @@
         <v>38</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>80</v>
+        <v>107</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I22" s="11"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="7"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1181,21 +1178,21 @@
         <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>111</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>93</v>
+        <v>110</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1203,18 +1200,18 @@
         <v>12</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I24" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1222,9 +1219,9 @@
         <v>12</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I25" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J25" t="s">
@@ -1232,8 +1229,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
@@ -1241,9 +1238,9 @@
         <v>12</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J26" t="s">
@@ -1251,8 +1248,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1260,9 +1257,9 @@
         <v>47</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I27" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J27" t="s">
@@ -1270,8 +1267,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1279,23 +1276,23 @@
         <v>12</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I28" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I29" s="11"/>
+      <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="9"/>
+      <c r="A30" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="10"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1305,19 +1302,19 @@
       <c r="E30" t="s">
         <v>40</v>
       </c>
-      <c r="I30" s="11" t="s">
+      <c r="I30" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J30" t="s">
+        <v>92</v>
+      </c>
+      <c r="K30" t="s">
         <v>93</v>
       </c>
-      <c r="J30" t="s">
-        <v>93</v>
-      </c>
-      <c r="K30" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1327,19 +1324,19 @@
       <c r="E31" t="s">
         <v>40</v>
       </c>
-      <c r="I31" s="11" t="s">
-        <v>93</v>
+      <c r="I31" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="J31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="1" t="s">
         <v>50</v>
       </c>
@@ -1347,26 +1344,26 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F32" s="6">
         <v>0</v>
       </c>
-      <c r="I32" s="12" t="s">
-        <v>80</v>
+      <c r="I32" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I33" s="11"/>
+      <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="1" t="s">
         <v>53</v>
       </c>
@@ -1376,19 +1373,19 @@
       <c r="E34" t="s">
         <v>9</v>
       </c>
-      <c r="I34" s="11" t="s">
+      <c r="I34" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" t="s">
         <v>87</v>
       </c>
-      <c r="J34" t="s">
-        <v>88</v>
-      </c>
       <c r="K34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="1" t="s">
         <v>54</v>
       </c>
@@ -1396,21 +1393,21 @@
         <v>55</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" t="s">
         <v>87</v>
       </c>
-      <c r="J35" t="s">
-        <v>88</v>
-      </c>
       <c r="K35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="1" t="s">
         <v>20</v>
       </c>
@@ -1421,26 +1418,26 @@
         <v>51</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I36" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K36" t="s">
         <v>93</v>
       </c>
-      <c r="J36" t="s">
-        <v>93</v>
-      </c>
-      <c r="K36" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I37" s="11"/>
+      <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="7"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
@@ -1454,21 +1451,21 @@
         <v>64</v>
       </c>
       <c r="H38" t="s">
-        <v>112</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>93</v>
+        <v>111</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1478,10 +1475,7 @@
       <c r="E39" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I39" s="11" t="s">
+      <c r="I39" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J39" t="s">
@@ -1489,8 +1483,8 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="1" t="s">
         <v>58</v>
       </c>
@@ -1498,9 +1492,9 @@
         <v>28</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I40" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J40" t="s">
@@ -1508,8 +1502,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="1" t="s">
         <v>59</v>
       </c>
@@ -1517,18 +1511,18 @@
         <v>55</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I41" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="1" t="s">
         <v>60</v>
       </c>
@@ -1536,18 +1530,18 @@
         <v>55</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I42" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I42" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="1" t="s">
         <v>61</v>
       </c>
@@ -1555,9 +1549,9 @@
         <v>28</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I43" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J43" t="s">
@@ -1565,8 +1559,8 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1574,9 +1568,9 @@
         <v>28</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I44" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I44" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J44" t="s">
@@ -1584,8 +1578,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="1" t="s">
         <v>62</v>
       </c>
@@ -1593,9 +1587,9 @@
         <v>63</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I45" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I45" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J45" t="s">
@@ -1603,8 +1597,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="1" t="s">
         <v>20</v>
       </c>
@@ -1615,18 +1609,18 @@
         <v>51</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I46" s="11"/>
+        <v>107</v>
+      </c>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I47" s="11"/>
+      <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="1" t="s">
         <v>66</v>
       </c>
@@ -1637,24 +1631,24 @@
         <v>9</v>
       </c>
       <c r="G48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H48" t="s">
-        <v>113</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>93</v>
+        <v>112</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="1" t="s">
         <v>67</v>
       </c>
@@ -1662,21 +1656,21 @@
         <v>28</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>93</v>
+        <v>107</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
       <c r="C50" s="1" t="s">
         <v>68</v>
       </c>
@@ -1684,18 +1678,18 @@
         <v>28</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>72</v>
+        <v>107</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
       <c r="C51" s="1" t="s">
         <v>69</v>
       </c>
@@ -1703,69 +1697,72 @@
         <v>28</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I51" s="12" t="s">
-        <v>72</v>
+        <v>107</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
       <c r="C52" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>51</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>72</v>
+        <v>107</v>
+      </c>
+      <c r="I52" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>70</v>
+        <v>92</v>
+      </c>
+      <c r="K52" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="I53" s="8"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" t="s">
         <v>11</v>
       </c>
-      <c r="E53" t="s">
-        <v>51</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I53" s="12" t="s">
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J54" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" t="s">
         <v>93</v>
       </c>
-      <c r="J53" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="K53" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="7"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
       <c r="C55" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -1773,93 +1770,71 @@
       <c r="E55" t="s">
         <v>40</v>
       </c>
-      <c r="I55" s="11" t="s">
-        <v>93</v>
+      <c r="I55" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="J55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K55" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
       <c r="C56" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>40</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>93</v>
+        <v>74</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="J56" t="s">
-        <v>93</v>
-      </c>
-      <c r="K56" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="11"/>
       <c r="C57" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I57" s="11" t="s">
-        <v>72</v>
+        <v>108</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="J57" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58" t="s">
-        <v>75</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J58" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A30:B32"/>
-    <mergeCell ref="A34:B36"/>
-    <mergeCell ref="A38:B46"/>
-    <mergeCell ref="A48:B53"/>
-    <mergeCell ref="A55:B58"/>
     <mergeCell ref="A23:B28"/>
     <mergeCell ref="A3:B7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B16"/>
     <mergeCell ref="A18:B21"/>
+    <mergeCell ref="A30:B32"/>
+    <mergeCell ref="A34:B36"/>
+    <mergeCell ref="A38:B46"/>
+    <mergeCell ref="A48:B52"/>
+    <mergeCell ref="A54:B57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More progress on documentation, and fixed a major error in the Booking data, db scripts updated to match
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="117">
   <si>
     <t>Entity</t>
   </si>
@@ -355,6 +355,18 @@
   </si>
   <si>
     <t>EVENT_SEQ</t>
+  </si>
+  <si>
+    <t>BookingID</t>
+  </si>
+  <si>
+    <t>Foreign Key, Not Null</t>
+  </si>
+  <si>
+    <t>BOOKING_TRIG</t>
+  </si>
+  <si>
+    <t>BOOKING_SEQ</t>
   </si>
 </sst>
 </file>
@@ -425,13 +437,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,11 +746,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,10 +769,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -793,10 +805,10 @@
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -823,8 +835,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
@@ -842,8 +854,8 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
@@ -861,8 +873,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
@@ -880,8 +892,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
@@ -902,10 +914,10 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
@@ -932,8 +944,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
@@ -951,8 +963,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
@@ -970,8 +982,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
@@ -989,8 +1001,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
@@ -1008,8 +1020,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1030,8 +1042,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1052,8 +1064,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
@@ -1077,10 +1089,10 @@
       <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="11"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
@@ -1101,8 +1113,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="1" t="s">
         <v>35</v>
       </c>
@@ -1120,8 +1132,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1139,8 +1151,8 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
@@ -1161,10 +1173,10 @@
       <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="11"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1191,8 +1203,8 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1210,8 +1222,8 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
@@ -1229,8 +1241,8 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
@@ -1248,8 +1260,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1267,8 +1279,8 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1289,10 +1301,10 @@
       <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="10"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1313,8 +1325,8 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1335,8 +1347,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="1" t="s">
         <v>50</v>
       </c>
@@ -1360,10 +1372,10 @@
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="11"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="1" t="s">
         <v>53</v>
       </c>
@@ -1384,8 +1396,8 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="1" t="s">
         <v>54</v>
       </c>
@@ -1406,8 +1418,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="1" t="s">
         <v>20</v>
       </c>
@@ -1434,10 +1446,10 @@
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="11"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
@@ -1464,8 +1476,8 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="1" t="s">
         <v>43</v>
       </c>
@@ -1483,8 +1495,8 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="1" t="s">
         <v>58</v>
       </c>
@@ -1502,8 +1514,8 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="1" t="s">
         <v>59</v>
       </c>
@@ -1521,8 +1533,8 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="1" t="s">
         <v>60</v>
       </c>
@@ -1540,8 +1552,8 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="1" t="s">
         <v>61</v>
       </c>
@@ -1559,8 +1571,8 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="1" t="s">
         <v>5</v>
       </c>
@@ -1578,8 +1590,8 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
-      <c r="B45" s="11"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="1" t="s">
         <v>62</v>
       </c>
@@ -1597,8 +1609,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="1" t="s">
         <v>20</v>
       </c>
@@ -1617,10 +1629,10 @@
       <c r="I47" s="8"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="11"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="1" t="s">
         <v>66</v>
       </c>
@@ -1647,8 +1659,8 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="1" t="s">
         <v>67</v>
       </c>
@@ -1669,8 +1681,8 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
       <c r="C50" s="1" t="s">
         <v>68</v>
       </c>
@@ -1688,8 +1700,8 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="1" t="s">
         <v>69</v>
       </c>
@@ -1707,8 +1719,8 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="1" t="s">
         <v>57</v>
       </c>
@@ -1735,18 +1747,24 @@
       <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B54" s="11"/>
+      <c r="B54" s="10"/>
       <c r="C54" s="1" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>9</v>
+      </c>
+      <c r="G54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H54" t="s">
+        <v>116</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>92</v>
@@ -1755,20 +1773,20 @@
         <v>92</v>
       </c>
       <c r="K54" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
       <c r="C55" s="1" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>92</v>
@@ -1777,33 +1795,36 @@
         <v>92</v>
       </c>
       <c r="K55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>114</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J56" t="s">
+        <v>92</v>
+      </c>
+      <c r="K56" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="1" t="s">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D56" t="s">
-        <v>74</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I56" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J56" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="D57" t="s">
         <v>74</v>
@@ -1815,26 +1836,45 @@
         <v>71</v>
       </c>
       <c r="J57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A54:B58"/>
+    <mergeCell ref="A30:B32"/>
+    <mergeCell ref="A34:B36"/>
+    <mergeCell ref="A38:B46"/>
+    <mergeCell ref="A48:B52"/>
     <mergeCell ref="A23:B28"/>
     <mergeCell ref="A3:B7"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A9:B16"/>
     <mergeCell ref="A18:B21"/>
-    <mergeCell ref="A30:B32"/>
-    <mergeCell ref="A34:B36"/>
-    <mergeCell ref="A38:B46"/>
-    <mergeCell ref="A48:B52"/>
-    <mergeCell ref="A54:B57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished data mapping document
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -243,9 +243,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Source table</t>
-  </si>
-  <si>
     <t>Buildings</t>
   </si>
   <si>
@@ -321,12 +318,6 @@
     <t>FK from event database table</t>
   </si>
   <si>
-    <t>Start time</t>
-  </si>
-  <si>
-    <t>End time</t>
-  </si>
-  <si>
     <t>Equipment    Allocation</t>
   </si>
   <si>
@@ -367,6 +358,15 @@
   </si>
   <si>
     <t>BOOKING_SEQ</t>
+  </si>
+  <si>
+    <t>Source Excel Sheet</t>
+  </si>
+  <si>
+    <t>Start time/Booking Date</t>
+  </si>
+  <si>
+    <t>End time/Booking Date</t>
   </si>
 </sst>
 </file>
@@ -439,11 +439,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -750,7 +750,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J64" sqref="J64"/>
+      <selection pane="bottomLeft" activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,21 +758,21 @@
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="6" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
     <col min="10" max="10" width="29.5703125" customWidth="1"/>
     <col min="11" max="11" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
@@ -783,7 +783,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>15</v>
@@ -792,10 +792,10 @@
         <v>17</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>31</v>
@@ -825,13 +825,13 @@
         <v>18</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>39</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
         <v>2</v>
@@ -863,10 +863,10 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J5" t="s">
         <v>4</v>
@@ -882,10 +882,10 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
@@ -901,13 +901,13 @@
         <v>13</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -934,13 +934,13 @@
         <v>49</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -953,10 +953,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -972,13 +972,13 @@
         <v>28</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" t="s">
         <v>79</v>
-      </c>
-      <c r="J11" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -991,10 +991,10 @@
         <v>29</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
@@ -1010,10 +1010,10 @@
         <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
         <v>24</v>
@@ -1029,13 +1029,13 @@
         <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>25</v>
@@ -1051,13 +1051,13 @@
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>26</v>
@@ -1076,10 +1076,10 @@
         <v>32</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>2</v>
@@ -1103,13 +1103,13 @@
         <v>40</v>
       </c>
       <c r="I18" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" t="s">
         <v>92</v>
-      </c>
-      <c r="J18" t="s">
-        <v>92</v>
-      </c>
-      <c r="K18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1122,13 +1122,13 @@
         <v>38</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1141,13 +1141,13 @@
         <v>38</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1160,13 +1160,13 @@
         <v>38</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1190,16 +1190,16 @@
         <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1212,13 +1212,13 @@
         <v>12</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1231,7 +1231,7 @@
         <v>12</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>41</v>
@@ -1250,7 +1250,7 @@
         <v>12</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>41</v>
@@ -1269,7 +1269,7 @@
         <v>47</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>41</v>
@@ -1288,23 +1288,23 @@
         <v>12</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>41</v>
       </c>
       <c r="J28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="12"/>
+      <c r="A30" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="11"/>
       <c r="C30" s="1" t="s">
         <v>20</v>
       </c>
@@ -1315,18 +1315,18 @@
         <v>40</v>
       </c>
       <c r="I30" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J30" t="s">
+        <v>91</v>
+      </c>
+      <c r="K30" t="s">
         <v>92</v>
       </c>
-      <c r="J30" t="s">
-        <v>92</v>
-      </c>
-      <c r="K30" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1337,18 +1337,18 @@
         <v>40</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="1" t="s">
         <v>50</v>
       </c>
@@ -1356,13 +1356,13 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F32" s="6">
         <v>0</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>50</v>
@@ -1386,13 +1386,13 @@
         <v>9</v>
       </c>
       <c r="I34" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34" t="s">
         <v>86</v>
       </c>
-      <c r="J34" t="s">
-        <v>87</v>
-      </c>
       <c r="K34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1405,16 +1405,16 @@
         <v>55</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I35" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J35" t="s">
         <v>86</v>
       </c>
-      <c r="J35" t="s">
-        <v>87</v>
-      </c>
       <c r="K35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1430,16 +1430,16 @@
         <v>51</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I36" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" t="s">
         <v>92</v>
-      </c>
-      <c r="J36" t="s">
-        <v>92</v>
-      </c>
-      <c r="K36" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1463,16 +1463,16 @@
         <v>64</v>
       </c>
       <c r="H38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I38" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>28</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I40" s="8" t="s">
         <v>56</v>
@@ -1523,13 +1523,13 @@
         <v>55</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I41" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1542,13 +1542,13 @@
         <v>55</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>56</v>
       </c>
       <c r="J42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>28</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>56</v>
@@ -1580,7 +1580,7 @@
         <v>28</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>56</v>
@@ -1599,7 +1599,7 @@
         <v>63</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>56</v>
@@ -1621,7 +1621,7 @@
         <v>51</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I46" s="8"/>
     </row>
@@ -1646,16 +1646,16 @@
         <v>70</v>
       </c>
       <c r="H48" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I48" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -1668,16 +1668,16 @@
         <v>28</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I49" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -1690,13 +1690,13 @@
         <v>28</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I50" s="9" t="s">
         <v>71</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>28</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I51" s="9" t="s">
         <v>71</v>
@@ -1731,16 +1731,16 @@
         <v>51</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
       </c>
       <c r="B54" s="10"/>
       <c r="C54" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -1761,19 +1761,19 @@
         <v>9</v>
       </c>
       <c r="G54" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H54" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -1786,16 +1786,16 @@
         <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I55" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J55" t="s">
+        <v>91</v>
+      </c>
+      <c r="K55" t="s">
         <v>92</v>
-      </c>
-      <c r="J55" t="s">
-        <v>92</v>
-      </c>
-      <c r="K55" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -1808,16 +1808,16 @@
         <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -1830,13 +1830,13 @@
         <v>74</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>71</v>
       </c>
       <c r="J57" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -1849,13 +1849,13 @@
         <v>74</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>71</v>
       </c>
       <c r="J58" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -1865,16 +1865,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A23:B28"/>
+    <mergeCell ref="A3:B7"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A9:B16"/>
+    <mergeCell ref="A18:B21"/>
     <mergeCell ref="A54:B58"/>
     <mergeCell ref="A30:B32"/>
     <mergeCell ref="A34:B36"/>
     <mergeCell ref="A38:B46"/>
     <mergeCell ref="A48:B52"/>
-    <mergeCell ref="A23:B28"/>
-    <mergeCell ref="A3:B7"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A9:B16"/>
-    <mergeCell ref="A18:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>